<commit_message>
interfaz para medir pesos
</commit_message>
<xml_diff>
--- a/SmartScale/assets/texts/texts.xlsx
+++ b/SmartScale/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14531" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71719" uniqueCount="539">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -565,6 +565,1383 @@
   </si>
   <si>
     <t xml:space="preserve">Manejo de usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget Wildcard Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu_main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empezar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estadísticas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estadisticas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanza
+Inteligente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador de los perfiles
+Por productos registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración general del
+dispositivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registros y valores obtenidos
+de los productos recientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de los usuarios
+del sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfil 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perfilesbtn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfil vacio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pesar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enviar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aire comp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogeno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00,00 [Kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promedio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERTA!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voler a pesar?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfil Vacio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%f&gt; [Kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;f&gt; [Kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;d&gt; [Kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00.00 [Kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;d&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volver a pesar?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione
+el perfil
+del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uidados intensivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Borrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfil incompleto!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso
+Esperado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencia
+Permitida</t>
   </si>
 </sst>
 </file>
@@ -1773,6 +3150,9 @@
       <c r="I3" s="20" t="s">
         <v>28</v>
       </c>
+      <c r="J3" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -1790,11 +3170,16 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
       <c r="H4" t="s">
         <v>74</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>377</v>
+      </c>
+      <c r="J4"/>
       <c r="K4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1827,9 +3212,14 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5"/>
-      <c r="H5"/>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
       <c r="I5"/>
+      <c r="J5"/>
       <c r="K5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1860,9 +3250,14 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6"/>
-      <c r="H6"/>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
       <c r="I6"/>
+      <c r="J6"/>
       <c r="K6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1893,9 +3288,14 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="G7"/>
-      <c r="H7"/>
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
       <c r="I7"/>
+      <c r="J7"/>
       <c r="K7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1935,6 +3335,7 @@
         <v>74</v>
       </c>
       <c r="I8"/>
+      <c r="J8"/>
       <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1972,6 +3373,7 @@
         <v>74</v>
       </c>
       <c r="I9"/>
+      <c r="J9"/>
       <c r="K9" s="11" t="s">
         <v>6</v>
       </c>
@@ -2011,6 +3413,7 @@
         <v>74</v>
       </c>
       <c r="I10"/>
+      <c r="J10"/>
       <c r="K10" s="11" t="s">
         <v>28</v>
       </c>
@@ -2044,6 +3447,7 @@
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
+      <c r="J11"/>
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="2:15">
@@ -2062,19 +3466,63 @@
       <c r="F12" t="s">
         <v>17</v>
       </c>
-      <c r="G12" t="s">
-        <v>73</v>
-      </c>
+      <c r="G12"/>
       <c r="H12" t="s">
         <v>74</v>
       </c>
       <c r="I12"/>
+      <c r="J12"/>
       <c r="L12" s="16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13">
+      <c r="B13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13"/>
       <c r="I13"/>
+      <c r="J13"/>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14"/>
+      <c r="J14"/>
     </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -2426,7 +3874,7 @@
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C21" t="s">
         <v>37</v>
@@ -2438,26 +3886,1234 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>181</v>
+      </c>
+      <c r="C30" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>205</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>207</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>208</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>211</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>324</v>
+      </c>
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>333</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>335</v>
+      </c>
+      <c r="C45" t="s">
+        <v>325</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>336</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>337</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>339</v>
+      </c>
+      <c r="C48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>341</v>
+      </c>
+      <c r="C49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>342</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>54</v>
+      </c>
+      <c r="E50" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>344</v>
+      </c>
+      <c r="C51" t="s">
+        <v>325</v>
+      </c>
+      <c r="D51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" t="s">
+        <v>43</v>
+      </c>
+      <c r="F51" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>346</v>
+      </c>
+      <c r="C52" t="s">
+        <v>325</v>
+      </c>
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>348</v>
+      </c>
+      <c r="C53" t="s">
+        <v>325</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F53" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>354</v>
+      </c>
+      <c r="C54" t="s">
+        <v>325</v>
+      </c>
+      <c r="D54" t="s">
+        <v>54</v>
+      </c>
+      <c r="E54" t="s">
+        <v>43</v>
+      </c>
+      <c r="F54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>355</v>
+      </c>
+      <c r="C55" t="s">
+        <v>325</v>
+      </c>
+      <c r="D55" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" t="s">
+        <v>43</v>
+      </c>
+      <c r="F55" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>356</v>
+      </c>
+      <c r="C56" t="s">
+        <v>325</v>
+      </c>
+      <c r="D56" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" t="s">
+        <v>43</v>
+      </c>
+      <c r="F56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>357</v>
+      </c>
+      <c r="C57" t="s">
+        <v>325</v>
+      </c>
+      <c r="D57" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" t="s">
+        <v>43</v>
+      </c>
+      <c r="F57" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>358</v>
+      </c>
+      <c r="C58" t="s">
+        <v>325</v>
+      </c>
+      <c r="D58" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58" t="s">
+        <v>43</v>
+      </c>
+      <c r="F58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>359</v>
+      </c>
+      <c r="C59" t="s">
+        <v>325</v>
+      </c>
+      <c r="D59" t="s">
+        <v>42</v>
+      </c>
+      <c r="E59" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>361</v>
+      </c>
+      <c r="C60" t="s">
+        <v>325</v>
+      </c>
+      <c r="D60" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" t="s">
+        <v>43</v>
+      </c>
+      <c r="F60" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>362</v>
+      </c>
+      <c r="C61" t="s">
+        <v>325</v>
+      </c>
+      <c r="D61" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" t="s">
+        <v>43</v>
+      </c>
+      <c r="F61" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>363</v>
+      </c>
+      <c r="C62" t="s">
+        <v>325</v>
+      </c>
+      <c r="D62" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62" t="s">
+        <v>43</v>
+      </c>
+      <c r="F62" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>364</v>
+      </c>
+      <c r="C63" t="s">
+        <v>325</v>
+      </c>
+      <c r="D63" t="s">
+        <v>42</v>
+      </c>
+      <c r="E63" t="s">
+        <v>43</v>
+      </c>
+      <c r="F63" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>365</v>
+      </c>
+      <c r="C64" t="s">
+        <v>325</v>
+      </c>
+      <c r="D64" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" t="s">
+        <v>43</v>
+      </c>
+      <c r="F64" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>368</v>
+      </c>
+      <c r="C65" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>375</v>
+      </c>
+      <c r="C66" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" t="s">
+        <v>42</v>
+      </c>
+      <c r="E66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>379</v>
+      </c>
+      <c r="C67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>380</v>
+      </c>
+      <c r="C68" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" t="s">
+        <v>42</v>
+      </c>
+      <c r="E68" t="s">
+        <v>43</v>
+      </c>
+      <c r="F68" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>382</v>
+      </c>
+      <c r="C69" t="s">
         <v>37</v>
       </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" t="s">
-        <v>165</v>
-      </c>
-    </row>
+      <c r="D69" t="s">
+        <v>54</v>
+      </c>
+      <c r="E69" t="s">
+        <v>43</v>
+      </c>
+      <c r="F69" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>384</v>
+      </c>
+      <c r="C70" t="s">
+        <v>37</v>
+      </c>
+      <c r="D70" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70" t="s">
+        <v>43</v>
+      </c>
+      <c r="F70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>398</v>
+      </c>
+      <c r="C71" t="s">
+        <v>325</v>
+      </c>
+      <c r="D71" t="s">
+        <v>54</v>
+      </c>
+      <c r="E71" t="s">
+        <v>43</v>
+      </c>
+      <c r="F71" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>399</v>
+      </c>
+      <c r="C72" t="s">
+        <v>325</v>
+      </c>
+      <c r="D72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E72" t="s">
+        <v>43</v>
+      </c>
+      <c r="F72" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>400</v>
+      </c>
+      <c r="C73" t="s">
+        <v>325</v>
+      </c>
+      <c r="D73" t="s">
+        <v>54</v>
+      </c>
+      <c r="E73" t="s">
+        <v>43</v>
+      </c>
+      <c r="F73" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>401</v>
+      </c>
+      <c r="C74" t="s">
+        <v>325</v>
+      </c>
+      <c r="D74" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" t="s">
+        <v>43</v>
+      </c>
+      <c r="F74" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>402</v>
+      </c>
+      <c r="C75" t="s">
+        <v>325</v>
+      </c>
+      <c r="D75" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75" t="s">
+        <v>43</v>
+      </c>
+      <c r="F75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>403</v>
+      </c>
+      <c r="C76" t="s">
+        <v>325</v>
+      </c>
+      <c r="D76" t="s">
+        <v>42</v>
+      </c>
+      <c r="E76" t="s">
+        <v>43</v>
+      </c>
+      <c r="F76" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>404</v>
+      </c>
+      <c r="C77" t="s">
+        <v>325</v>
+      </c>
+      <c r="D77" t="s">
+        <v>54</v>
+      </c>
+      <c r="E77" t="s">
+        <v>43</v>
+      </c>
+      <c r="F77" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>405</v>
+      </c>
+      <c r="C78" t="s">
+        <v>325</v>
+      </c>
+      <c r="D78" t="s">
+        <v>42</v>
+      </c>
+      <c r="E78" t="s">
+        <v>43</v>
+      </c>
+      <c r="F78" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>406</v>
+      </c>
+      <c r="C79" t="s">
+        <v>325</v>
+      </c>
+      <c r="D79" t="s">
+        <v>54</v>
+      </c>
+      <c r="E79" t="s">
+        <v>43</v>
+      </c>
+      <c r="F79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>407</v>
+      </c>
+      <c r="C80" t="s">
+        <v>325</v>
+      </c>
+      <c r="D80" t="s">
+        <v>42</v>
+      </c>
+      <c r="E80" t="s">
+        <v>43</v>
+      </c>
+      <c r="F80" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>408</v>
+      </c>
+      <c r="C81" t="s">
+        <v>37</v>
+      </c>
+      <c r="D81" t="s">
+        <v>42</v>
+      </c>
+      <c r="E81" t="s">
+        <v>43</v>
+      </c>
+      <c r="F81" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>409</v>
+      </c>
+      <c r="C82" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" t="s">
+        <v>42</v>
+      </c>
+      <c r="E82" t="s">
+        <v>43</v>
+      </c>
+      <c r="F82" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>411</v>
+      </c>
+      <c r="C83" t="s">
+        <v>50</v>
+      </c>
+      <c r="D83" t="s">
+        <v>54</v>
+      </c>
+      <c r="E83" t="s">
+        <v>43</v>
+      </c>
+      <c r="F83" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>413</v>
+      </c>
+      <c r="C84" t="s">
+        <v>40</v>
+      </c>
+      <c r="D84" t="s">
+        <v>42</v>
+      </c>
+      <c r="E84" t="s">
+        <v>43</v>
+      </c>
+      <c r="F84" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>414</v>
+      </c>
+      <c r="C85" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" t="s">
+        <v>54</v>
+      </c>
+      <c r="E85" t="s">
+        <v>43</v>
+      </c>
+      <c r="F85" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="s">
+        <v>416</v>
+      </c>
+      <c r="C86" t="s">
+        <v>50</v>
+      </c>
+      <c r="D86" t="s">
+        <v>54</v>
+      </c>
+      <c r="E86" t="s">
+        <v>43</v>
+      </c>
+      <c r="F86" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="s">
+        <v>417</v>
+      </c>
+      <c r="C87" t="s">
+        <v>40</v>
+      </c>
+      <c r="D87" t="s">
+        <v>42</v>
+      </c>
+      <c r="E87" t="s">
+        <v>43</v>
+      </c>
+      <c r="F87" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
+        <v>418</v>
+      </c>
+      <c r="C88" t="s">
+        <v>40</v>
+      </c>
+      <c r="D88" t="s">
+        <v>54</v>
+      </c>
+      <c r="E88" t="s">
+        <v>43</v>
+      </c>
+      <c r="F88" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="s">
+        <v>428</v>
+      </c>
+      <c r="C89" t="s">
+        <v>37</v>
+      </c>
+      <c r="D89" t="s">
+        <v>42</v>
+      </c>
+      <c r="E89" t="s">
+        <v>43</v>
+      </c>
+      <c r="F89" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="s">
+        <v>429</v>
+      </c>
+      <c r="C90" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" t="s">
+        <v>42</v>
+      </c>
+      <c r="E90" t="s">
+        <v>43</v>
+      </c>
+      <c r="F90" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
+        <v>495</v>
+      </c>
+      <c r="C91" t="s">
+        <v>50</v>
+      </c>
+      <c r="D91" t="s">
+        <v>42</v>
+      </c>
+      <c r="E91" t="s">
+        <v>43</v>
+      </c>
+      <c r="F91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="s">
+        <v>496</v>
+      </c>
+      <c r="C92" t="s">
+        <v>50</v>
+      </c>
+      <c r="D92" t="s">
+        <v>42</v>
+      </c>
+      <c r="E92" t="s">
+        <v>43</v>
+      </c>
+      <c r="F92" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="s">
+        <v>517</v>
+      </c>
+      <c r="C93" t="s">
+        <v>325</v>
+      </c>
+      <c r="D93" t="s">
+        <v>42</v>
+      </c>
+      <c r="E93" t="s">
+        <v>43</v>
+      </c>
+      <c r="F93" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="94"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
solo visualizar los perfiles
</commit_message>
<xml_diff>
--- a/SmartScale/assets/texts/texts.xlsx
+++ b/SmartScale/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71719" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109574" uniqueCount="630">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1942,6 +1942,347 @@
   <si>
     <t xml:space="preserve">Diferencia
 Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789 :APM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numPad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!”"#*%&amp;()'$+-@_, .:;?/~±×÷•º`´{}©£€^®¥_=[]¡¢|\¿&gt;&lt;áéíóú</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;d&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Información</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
   </si>
 </sst>
 </file>
@@ -3171,7 +3512,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H4" t="s">
         <v>74</v>
@@ -3213,7 +3554,7 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H5" t="s">
         <v>74</v>
@@ -3251,7 +3592,7 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H6" t="s">
         <v>74</v>
@@ -3289,7 +3630,7 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H7" t="s">
         <v>74</v>
@@ -3329,7 +3670,7 @@
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>161</v>
+        <v>552</v>
       </c>
       <c r="H8" t="s">
         <v>74</v>
@@ -3367,7 +3708,7 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H9" t="s">
         <v>74</v>
@@ -3407,7 +3748,7 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H10" t="s">
         <v>74</v>
@@ -3493,7 +3834,7 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -3516,7 +3857,7 @@
         <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H14" t="s">
         <v>74</v>
@@ -3585,10 +3926,10 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -3597,32 +3938,32 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -3631,15 +3972,15 @@
         <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>63</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
         <v>42</v>
@@ -3648,32 +3989,32 @@
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
@@ -3682,49 +4023,49 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="C10" t="s">
         <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>84</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
         <v>42</v>
@@ -3733,32 +4074,32 @@
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>91</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
         <v>42</v>
@@ -3767,15 +4108,15 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>98</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
         <v>42</v>
@@ -3784,49 +4125,49 @@
         <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>112</v>
+        <v>324</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>373</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>125</v>
+        <v>333</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>126</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>151</v>
+        <v>335</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>325</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -3835,15 +4176,15 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>156</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>152</v>
+        <v>336</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
@@ -3852,15 +4193,15 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>157</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>154</v>
+        <v>337</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>42</v>
@@ -3869,15 +4210,15 @@
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>155</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>163</v>
+        <v>339</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
@@ -3886,15 +4227,15 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>165</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>168</v>
+        <v>341</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
@@ -3903,15 +4244,15 @@
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>169</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>170</v>
+        <v>342</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
         <v>54</v>
@@ -3920,49 +4261,49 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>171</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>172</v>
+        <v>344</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>173</v>
+        <v>378</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>174</v>
+        <v>346</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>171</v>
+        <v>347</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>175</v>
+        <v>348</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D26" t="s">
         <v>42</v>
@@ -3971,15 +4312,15 @@
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>176</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>177</v>
+        <v>354</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D27" t="s">
         <v>54</v>
@@ -3988,32 +4329,32 @@
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>171</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>178</v>
+        <v>355</v>
       </c>
       <c r="C28" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>180</v>
+        <v>356</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D29" t="s">
         <v>54</v>
@@ -4022,32 +4363,32 @@
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>171</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>181</v>
+        <v>357</v>
       </c>
       <c r="C30" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>183</v>
+        <v>358</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D31" t="s">
         <v>54</v>
@@ -4056,32 +4397,32 @@
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>171</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>184</v>
+        <v>359</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E32" t="s">
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>186</v>
+        <v>361</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
@@ -4090,15 +4431,15 @@
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>187</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>188</v>
+        <v>362</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -4107,15 +4448,15 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>189</v>
+        <v>326</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>190</v>
+        <v>363</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
@@ -4124,15 +4465,15 @@
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>191</v>
+        <v>326</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>192</v>
+        <v>364</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D36" t="s">
         <v>42</v>
@@ -4141,15 +4482,15 @@
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>193</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>204</v>
+        <v>365</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>325</v>
       </c>
       <c r="D37" t="s">
         <v>42</v>
@@ -4158,15 +4499,15 @@
         <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>162</v>
+        <v>366</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>205</v>
+        <v>368</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D38" t="s">
         <v>42</v>
@@ -4175,15 +4516,15 @@
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>206</v>
+        <v>369</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>207</v>
+        <v>375</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
         <v>42</v>
@@ -4192,15 +4533,15 @@
         <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>173</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>208</v>
+        <v>379</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -4209,12 +4550,12 @@
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>176</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>209</v>
+        <v>380</v>
       </c>
       <c r="C41" t="s">
         <v>50</v>
@@ -4226,32 +4567,32 @@
         <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>210</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>211</v>
+        <v>382</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>182</v>
+        <v>383</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>324</v>
+        <v>384</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D43" t="s">
         <v>54</v>
@@ -4260,29 +4601,29 @@
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>373</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>333</v>
+        <v>398</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>325</v>
       </c>
       <c r="D44" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E44" t="s">
         <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>334</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>335</v>
+        <v>399</v>
       </c>
       <c r="C45" t="s">
         <v>325</v>
@@ -4294,32 +4635,32 @@
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>94</v>
+        <v>326</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>336</v>
+        <v>400</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D46" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E46" t="s">
         <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>334</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>337</v>
+        <v>401</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D47" t="s">
         <v>42</v>
@@ -4328,32 +4669,32 @@
         <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>371</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>339</v>
+        <v>402</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E48" t="s">
         <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>340</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>341</v>
+        <v>403</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D49" t="s">
         <v>42</v>
@@ -4362,15 +4703,15 @@
         <v>43</v>
       </c>
       <c r="F49" t="s">
-        <v>371</v>
+        <v>326</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>342</v>
+        <v>404</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>325</v>
       </c>
       <c r="D50" t="s">
         <v>54</v>
@@ -4379,46 +4720,46 @@
         <v>43</v>
       </c>
       <c r="F50" t="s">
-        <v>374</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>344</v>
+        <v>405</v>
       </c>
       <c r="C51" t="s">
         <v>325</v>
       </c>
       <c r="D51" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E51" t="s">
         <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>346</v>
+        <v>406</v>
       </c>
       <c r="C52" t="s">
         <v>325</v>
       </c>
       <c r="D52" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E52" t="s">
         <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>347</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>348</v>
+        <v>407</v>
       </c>
       <c r="C53" t="s">
         <v>325</v>
@@ -4430,32 +4771,32 @@
         <v>43</v>
       </c>
       <c r="F53" t="s">
-        <v>329</v>
+        <v>360</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>354</v>
+        <v>408</v>
       </c>
       <c r="C54" t="s">
-        <v>325</v>
+        <v>37</v>
       </c>
       <c r="D54" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E54" t="s">
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>94</v>
+        <v>374</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>355</v>
+        <v>411</v>
       </c>
       <c r="C55" t="s">
-        <v>325</v>
+        <v>50</v>
       </c>
       <c r="D55" t="s">
         <v>54</v>
@@ -4464,32 +4805,32 @@
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>94</v>
+        <v>374</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>356</v>
+        <v>413</v>
       </c>
       <c r="C56" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="D56" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E56" t="s">
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>94</v>
+        <v>347</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>357</v>
+        <v>414</v>
       </c>
       <c r="C57" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="D57" t="s">
         <v>54</v>
@@ -4498,15 +4839,15 @@
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>94</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>358</v>
+        <v>416</v>
       </c>
       <c r="C58" t="s">
-        <v>325</v>
+        <v>50</v>
       </c>
       <c r="D58" t="s">
         <v>54</v>
@@ -4515,15 +4856,15 @@
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>94</v>
+        <v>374</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>359</v>
+        <v>417</v>
       </c>
       <c r="C59" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="D59" t="s">
         <v>42</v>
@@ -4532,32 +4873,32 @@
         <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>361</v>
+        <v>418</v>
       </c>
       <c r="C60" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="D60" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E60" t="s">
         <v>43</v>
       </c>
       <c r="F60" t="s">
-        <v>360</v>
+        <v>419</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>362</v>
+        <v>428</v>
       </c>
       <c r="C61" t="s">
-        <v>325</v>
+        <v>37</v>
       </c>
       <c r="D61" t="s">
         <v>42</v>
@@ -4566,15 +4907,15 @@
         <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>326</v>
+        <v>360</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>363</v>
+        <v>495</v>
       </c>
       <c r="C62" t="s">
-        <v>325</v>
+        <v>50</v>
       </c>
       <c r="D62" t="s">
         <v>42</v>
@@ -4583,15 +4924,15 @@
         <v>43</v>
       </c>
       <c r="F62" t="s">
-        <v>326</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>364</v>
+        <v>496</v>
       </c>
       <c r="C63" t="s">
-        <v>325</v>
+        <v>50</v>
       </c>
       <c r="D63" t="s">
         <v>42</v>
@@ -4600,15 +4941,15 @@
         <v>43</v>
       </c>
       <c r="F63" t="s">
-        <v>326</v>
+        <v>369</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>365</v>
+        <v>409</v>
       </c>
       <c r="C64" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="D64" t="s">
         <v>42</v>
@@ -4617,12 +4958,12 @@
         <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>368</v>
+        <v>429</v>
       </c>
       <c r="C65" t="s">
         <v>40</v>
@@ -4634,15 +4975,15 @@
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>369</v>
+        <v>430</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>375</v>
+        <v>550</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s">
         <v>42</v>
@@ -4651,63 +4992,63 @@
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>327</v>
+        <v>555</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>379</v>
+        <v>556</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D67" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E67" t="s">
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>369</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>380</v>
+        <v>596</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D68" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E68" t="s">
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>381</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>382</v>
+        <v>597</v>
       </c>
       <c r="C69" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="D69" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E69" t="s">
         <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>383</v>
+        <v>598</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>384</v>
+        <v>605</v>
       </c>
       <c r="C70" t="s">
         <v>37</v>
@@ -4719,15 +5060,15 @@
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>126</v>
+        <v>606</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>398</v>
+        <v>607</v>
       </c>
       <c r="C71" t="s">
-        <v>325</v>
+        <v>37</v>
       </c>
       <c r="D71" t="s">
         <v>54</v>
@@ -4736,383 +5077,31 @@
         <v>43</v>
       </c>
       <c r="F71" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="B72" t="s">
-        <v>399</v>
-      </c>
-      <c r="C72" t="s">
-        <v>325</v>
-      </c>
-      <c r="D72" t="s">
-        <v>42</v>
-      </c>
-      <c r="E72" t="s">
-        <v>43</v>
-      </c>
-      <c r="F72" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="B73" t="s">
-        <v>400</v>
-      </c>
-      <c r="C73" t="s">
-        <v>325</v>
-      </c>
-      <c r="D73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E73" t="s">
-        <v>43</v>
-      </c>
-      <c r="F73" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="B74" t="s">
-        <v>401</v>
-      </c>
-      <c r="C74" t="s">
-        <v>325</v>
-      </c>
-      <c r="D74" t="s">
-        <v>42</v>
-      </c>
-      <c r="E74" t="s">
-        <v>43</v>
-      </c>
-      <c r="F74" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" t="s">
-        <v>402</v>
-      </c>
-      <c r="C75" t="s">
-        <v>325</v>
-      </c>
-      <c r="D75" t="s">
-        <v>54</v>
-      </c>
-      <c r="E75" t="s">
-        <v>43</v>
-      </c>
-      <c r="F75" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" t="s">
-        <v>403</v>
-      </c>
-      <c r="C76" t="s">
-        <v>325</v>
-      </c>
-      <c r="D76" t="s">
-        <v>42</v>
-      </c>
-      <c r="E76" t="s">
-        <v>43</v>
-      </c>
-      <c r="F76" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" t="s">
-        <v>404</v>
-      </c>
-      <c r="C77" t="s">
-        <v>325</v>
-      </c>
-      <c r="D77" t="s">
-        <v>54</v>
-      </c>
-      <c r="E77" t="s">
-        <v>43</v>
-      </c>
-      <c r="F77" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" t="s">
-        <v>405</v>
-      </c>
-      <c r="C78" t="s">
-        <v>325</v>
-      </c>
-      <c r="D78" t="s">
-        <v>42</v>
-      </c>
-      <c r="E78" t="s">
-        <v>43</v>
-      </c>
-      <c r="F78" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="B79" t="s">
-        <v>406</v>
-      </c>
-      <c r="C79" t="s">
-        <v>325</v>
-      </c>
-      <c r="D79" t="s">
-        <v>54</v>
-      </c>
-      <c r="E79" t="s">
-        <v>43</v>
-      </c>
-      <c r="F79" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="B80" t="s">
-        <v>407</v>
-      </c>
-      <c r="C80" t="s">
-        <v>325</v>
-      </c>
-      <c r="D80" t="s">
-        <v>42</v>
-      </c>
-      <c r="E80" t="s">
-        <v>43</v>
-      </c>
-      <c r="F80" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="B81" t="s">
-        <v>408</v>
-      </c>
-      <c r="C81" t="s">
-        <v>37</v>
-      </c>
-      <c r="D81" t="s">
-        <v>42</v>
-      </c>
-      <c r="E81" t="s">
-        <v>43</v>
-      </c>
-      <c r="F81" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="B82" t="s">
-        <v>409</v>
-      </c>
-      <c r="C82" t="s">
-        <v>40</v>
-      </c>
-      <c r="D82" t="s">
-        <v>42</v>
-      </c>
-      <c r="E82" t="s">
-        <v>43</v>
-      </c>
-      <c r="F82" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="B83" t="s">
-        <v>411</v>
-      </c>
-      <c r="C83" t="s">
-        <v>50</v>
-      </c>
-      <c r="D83" t="s">
-        <v>54</v>
-      </c>
-      <c r="E83" t="s">
-        <v>43</v>
-      </c>
-      <c r="F83" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="B84" t="s">
-        <v>413</v>
-      </c>
-      <c r="C84" t="s">
-        <v>40</v>
-      </c>
-      <c r="D84" t="s">
-        <v>42</v>
-      </c>
-      <c r="E84" t="s">
-        <v>43</v>
-      </c>
-      <c r="F84" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="B85" t="s">
-        <v>414</v>
-      </c>
-      <c r="C85" t="s">
-        <v>40</v>
-      </c>
-      <c r="D85" t="s">
-        <v>54</v>
-      </c>
-      <c r="E85" t="s">
-        <v>43</v>
-      </c>
-      <c r="F85" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="B86" t="s">
-        <v>416</v>
-      </c>
-      <c r="C86" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" t="s">
-        <v>54</v>
-      </c>
-      <c r="E86" t="s">
-        <v>43</v>
-      </c>
-      <c r="F86" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="B87" t="s">
-        <v>417</v>
-      </c>
-      <c r="C87" t="s">
-        <v>40</v>
-      </c>
-      <c r="D87" t="s">
-        <v>42</v>
-      </c>
-      <c r="E87" t="s">
-        <v>43</v>
-      </c>
-      <c r="F87" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="B88" t="s">
-        <v>418</v>
-      </c>
-      <c r="C88" t="s">
-        <v>40</v>
-      </c>
-      <c r="D88" t="s">
-        <v>54</v>
-      </c>
-      <c r="E88" t="s">
-        <v>43</v>
-      </c>
-      <c r="F88" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="B89" t="s">
-        <v>428</v>
-      </c>
-      <c r="C89" t="s">
-        <v>37</v>
-      </c>
-      <c r="D89" t="s">
-        <v>42</v>
-      </c>
-      <c r="E89" t="s">
-        <v>43</v>
-      </c>
-      <c r="F89" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="B90" t="s">
-        <v>429</v>
-      </c>
-      <c r="C90" t="s">
-        <v>40</v>
-      </c>
-      <c r="D90" t="s">
-        <v>42</v>
-      </c>
-      <c r="E90" t="s">
-        <v>43</v>
-      </c>
-      <c r="F90" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="B91" t="s">
-        <v>495</v>
-      </c>
-      <c r="C91" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" t="s">
-        <v>42</v>
-      </c>
-      <c r="E91" t="s">
-        <v>43</v>
-      </c>
-      <c r="F91" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="B92" t="s">
-        <v>496</v>
-      </c>
-      <c r="C92" t="s">
-        <v>50</v>
-      </c>
-      <c r="D92" t="s">
-        <v>42</v>
-      </c>
-      <c r="E92" t="s">
-        <v>43</v>
-      </c>
-      <c r="F92" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="B93" t="s">
-        <v>517</v>
-      </c>
-      <c r="C93" t="s">
-        <v>325</v>
-      </c>
-      <c r="D93" t="s">
-        <v>42</v>
-      </c>
-      <c r="E93" t="s">
-        <v>43</v>
-      </c>
-      <c r="F93" t="s">
-        <v>518</v>
-      </c>
-    </row>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
     <row r="94"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
se agrego el numpad para modificar numeros
</commit_message>
<xml_diff>
--- a/SmartScale/assets/texts/texts.xlsx
+++ b/SmartScale/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109574" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109616" uniqueCount="630">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -4946,13 +4946,13 @@
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>409</v>
+        <v>517</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="D64" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E64" t="s">
         <v>43</v>
@@ -4963,10 +4963,10 @@
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>429</v>
+        <v>541</v>
       </c>
       <c r="C65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D65" t="s">
         <v>42</v>
@@ -4975,15 +4975,15 @@
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>430</v>
+        <v>373</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="C66" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D66" t="s">
         <v>42</v>
@@ -4992,49 +4992,49 @@
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="C67" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D67" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E67" t="s">
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>126</v>
+        <v>373</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>596</v>
+        <v>546</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="D68" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E68" t="s">
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>185</v>
+        <v>547</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>597</v>
+        <v>548</v>
       </c>
       <c r="C69" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="D69" t="s">
         <v>42</v>
@@ -5043,50 +5043,162 @@
         <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>598</v>
+        <v>542</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>605</v>
+        <v>549</v>
       </c>
       <c r="C70" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D70" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E70" t="s">
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>606</v>
+        <v>554</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
+        <v>409</v>
+      </c>
+      <c r="C71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" t="s">
+        <v>42</v>
+      </c>
+      <c r="E71" t="s">
+        <v>43</v>
+      </c>
+      <c r="F71" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>429</v>
+      </c>
+      <c r="C72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E72" t="s">
+        <v>43</v>
+      </c>
+      <c r="F72" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>550</v>
+      </c>
+      <c r="C73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D73" t="s">
+        <v>42</v>
+      </c>
+      <c r="E73" t="s">
+        <v>43</v>
+      </c>
+      <c r="F73" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>556</v>
+      </c>
+      <c r="C74" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" t="s">
+        <v>54</v>
+      </c>
+      <c r="E74" t="s">
+        <v>43</v>
+      </c>
+      <c r="F74" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C75" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75" t="s">
+        <v>43</v>
+      </c>
+      <c r="F75" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>597</v>
+      </c>
+      <c r="C76" t="s">
+        <v>167</v>
+      </c>
+      <c r="D76" t="s">
+        <v>42</v>
+      </c>
+      <c r="E76" t="s">
+        <v>43</v>
+      </c>
+      <c r="F76" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>605</v>
+      </c>
+      <c r="C77" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" t="s">
+        <v>54</v>
+      </c>
+      <c r="E77" t="s">
+        <v>43</v>
+      </c>
+      <c r="F77" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
         <v>607</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C78" t="s">
         <v>37</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D78" t="s">
         <v>54</v>
       </c>
-      <c r="E71" t="s">
-        <v>43</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E78" t="s">
+        <v>43</v>
+      </c>
+      <c r="F78" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
     <row r="79"/>
     <row r="80"/>
     <row r="81"/>

</xml_diff>

<commit_message>
ventana de peso completo
</commit_message>
<xml_diff>
--- a/SmartScale/assets/texts/texts.xlsx
+++ b/SmartScale/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71719" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109889" uniqueCount="630">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1942,6 +1942,347 @@
   <si>
     <t xml:space="preserve">Diferencia
 Permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789 :APM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numPad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!”"#*%&amp;()'$+-@_, .:;?/~±×÷•º`´{}©£€^®¥_=[]¡¢|\¿&gt;&lt;áéíóú</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;d&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Información</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Perfil esta 
+incompleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se envio el
+registro con éxito</t>
   </si>
 </sst>
 </file>
@@ -3171,7 +3512,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H4" t="s">
         <v>74</v>
@@ -3213,7 +3554,7 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H5" t="s">
         <v>74</v>
@@ -3251,7 +3592,7 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H6" t="s">
         <v>74</v>
@@ -3289,7 +3630,7 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H7" t="s">
         <v>74</v>
@@ -3329,7 +3670,7 @@
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>161</v>
+        <v>552</v>
       </c>
       <c r="H8" t="s">
         <v>74</v>
@@ -3367,7 +3708,7 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H9" t="s">
         <v>74</v>
@@ -3407,7 +3748,7 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H10" t="s">
         <v>74</v>
@@ -3493,7 +3834,7 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -3516,7 +3857,7 @@
         <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>552</v>
       </c>
       <c r="H14" t="s">
         <v>74</v>
@@ -3585,10 +3926,10 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -3597,32 +3938,32 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -3631,15 +3972,15 @@
         <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>63</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
         <v>42</v>
@@ -3648,32 +3989,32 @@
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
@@ -3682,49 +4023,49 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="C10" t="s">
         <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>84</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
         <v>42</v>
@@ -3733,32 +4074,32 @@
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>91</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
         <v>42</v>
@@ -3767,32 +4108,32 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>98</v>
+        <v>324</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
         <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>112</v>
+        <v>333</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
         <v>42</v>
@@ -3801,32 +4142,32 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>125</v>
+        <v>335</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>325</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>151</v>
+        <v>336</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -3835,15 +4176,15 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>156</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>152</v>
+        <v>337</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
@@ -3852,15 +4193,15 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>157</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>154</v>
+        <v>339</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>42</v>
@@ -3869,15 +4210,15 @@
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>155</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>163</v>
+        <v>341</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
@@ -3886,32 +4227,32 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>165</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>168</v>
+        <v>342</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>169</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>170</v>
+        <v>344</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D23" t="s">
         <v>54</v>
@@ -3920,15 +4261,15 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>171</v>
+        <v>378</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>172</v>
+        <v>346</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -3937,49 +4278,49 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>173</v>
+        <v>347</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>174</v>
+        <v>348</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>171</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>175</v>
+        <v>354</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>176</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>177</v>
+        <v>355</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D27" t="s">
         <v>54</v>
@@ -3988,32 +4329,32 @@
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>171</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>178</v>
+        <v>356</v>
       </c>
       <c r="C28" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>180</v>
+        <v>357</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D29" t="s">
         <v>54</v>
@@ -4022,66 +4363,66 @@
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>171</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>181</v>
+        <v>358</v>
       </c>
       <c r="C30" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>183</v>
+        <v>359</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>171</v>
+        <v>360</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>184</v>
+        <v>361</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E32" t="s">
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>186</v>
+        <v>362</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
@@ -4090,15 +4431,15 @@
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>187</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>188</v>
+        <v>363</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -4107,15 +4448,15 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>189</v>
+        <v>326</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>190</v>
+        <v>364</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
@@ -4124,15 +4465,15 @@
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>191</v>
+        <v>326</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>192</v>
+        <v>365</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D36" t="s">
         <v>42</v>
@@ -4141,15 +4482,15 @@
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>193</v>
+        <v>366</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>204</v>
+        <v>368</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
         <v>42</v>
@@ -4158,15 +4499,15 @@
         <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>162</v>
+        <v>369</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>205</v>
+        <v>375</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
         <v>42</v>
@@ -4175,15 +4516,15 @@
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>206</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>207</v>
+        <v>379</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D39" t="s">
         <v>42</v>
@@ -4192,12 +4533,12 @@
         <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>173</v>
+        <v>369</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>208</v>
+        <v>380</v>
       </c>
       <c r="C40" t="s">
         <v>50</v>
@@ -4209,49 +4550,49 @@
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>176</v>
+        <v>381</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>209</v>
+        <v>382</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E41" t="s">
         <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>210</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>211</v>
+        <v>384</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>182</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>324</v>
+        <v>596</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="D43" t="s">
         <v>54</v>
@@ -4260,15 +4601,15 @@
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>373</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>333</v>
+        <v>597</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>167</v>
       </c>
       <c r="D44" t="s">
         <v>42</v>
@@ -4277,842 +4618,90 @@
         <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>334</v>
+        <v>598</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>335</v>
+        <v>605</v>
       </c>
       <c r="C45" t="s">
-        <v>325</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E45" t="s">
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>94</v>
+        <v>606</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>336</v>
+        <v>607</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E46" t="s">
         <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="s">
-        <v>337</v>
-      </c>
-      <c r="C47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" t="s">
-        <v>43</v>
-      </c>
-      <c r="F47" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" t="s">
-        <v>339</v>
-      </c>
-      <c r="C48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" t="s">
-        <v>43</v>
-      </c>
-      <c r="F48" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="s">
-        <v>341</v>
-      </c>
-      <c r="C49" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" t="s">
-        <v>42</v>
-      </c>
-      <c r="E49" t="s">
-        <v>43</v>
-      </c>
-      <c r="F49" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="s">
-        <v>342</v>
-      </c>
-      <c r="C50" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" t="s">
-        <v>54</v>
-      </c>
-      <c r="E50" t="s">
-        <v>43</v>
-      </c>
-      <c r="F50" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="s">
-        <v>344</v>
-      </c>
-      <c r="C51" t="s">
-        <v>325</v>
-      </c>
-      <c r="D51" t="s">
-        <v>54</v>
-      </c>
-      <c r="E51" t="s">
-        <v>43</v>
-      </c>
-      <c r="F51" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" t="s">
-        <v>346</v>
-      </c>
-      <c r="C52" t="s">
-        <v>325</v>
-      </c>
-      <c r="D52" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" t="s">
-        <v>348</v>
-      </c>
-      <c r="C53" t="s">
-        <v>325</v>
-      </c>
-      <c r="D53" t="s">
-        <v>42</v>
-      </c>
-      <c r="E53" t="s">
-        <v>43</v>
-      </c>
-      <c r="F53" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" t="s">
-        <v>354</v>
-      </c>
-      <c r="C54" t="s">
-        <v>325</v>
-      </c>
-      <c r="D54" t="s">
-        <v>54</v>
-      </c>
-      <c r="E54" t="s">
-        <v>43</v>
-      </c>
-      <c r="F54" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" t="s">
-        <v>355</v>
-      </c>
-      <c r="C55" t="s">
-        <v>325</v>
-      </c>
-      <c r="D55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E55" t="s">
-        <v>43</v>
-      </c>
-      <c r="F55" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" t="s">
-        <v>356</v>
-      </c>
-      <c r="C56" t="s">
-        <v>325</v>
-      </c>
-      <c r="D56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E56" t="s">
-        <v>43</v>
-      </c>
-      <c r="F56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C57" t="s">
-        <v>325</v>
-      </c>
-      <c r="D57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E57" t="s">
-        <v>43</v>
-      </c>
-      <c r="F57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" t="s">
-        <v>358</v>
-      </c>
-      <c r="C58" t="s">
-        <v>325</v>
-      </c>
-      <c r="D58" t="s">
-        <v>54</v>
-      </c>
-      <c r="E58" t="s">
-        <v>43</v>
-      </c>
-      <c r="F58" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="B59" t="s">
-        <v>359</v>
-      </c>
-      <c r="C59" t="s">
-        <v>325</v>
-      </c>
-      <c r="D59" t="s">
-        <v>42</v>
-      </c>
-      <c r="E59" t="s">
-        <v>43</v>
-      </c>
-      <c r="F59" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" t="s">
-        <v>361</v>
-      </c>
-      <c r="C60" t="s">
-        <v>325</v>
-      </c>
-      <c r="D60" t="s">
-        <v>42</v>
-      </c>
-      <c r="E60" t="s">
-        <v>43</v>
-      </c>
-      <c r="F60" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="B61" t="s">
-        <v>362</v>
-      </c>
-      <c r="C61" t="s">
-        <v>325</v>
-      </c>
-      <c r="D61" t="s">
-        <v>42</v>
-      </c>
-      <c r="E61" t="s">
-        <v>43</v>
-      </c>
-      <c r="F61" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="B62" t="s">
-        <v>363</v>
-      </c>
-      <c r="C62" t="s">
-        <v>325</v>
-      </c>
-      <c r="D62" t="s">
-        <v>42</v>
-      </c>
-      <c r="E62" t="s">
-        <v>43</v>
-      </c>
-      <c r="F62" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="B63" t="s">
-        <v>364</v>
-      </c>
-      <c r="C63" t="s">
-        <v>325</v>
-      </c>
-      <c r="D63" t="s">
-        <v>42</v>
-      </c>
-      <c r="E63" t="s">
-        <v>43</v>
-      </c>
-      <c r="F63" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" t="s">
-        <v>365</v>
-      </c>
-      <c r="C64" t="s">
-        <v>325</v>
-      </c>
-      <c r="D64" t="s">
-        <v>42</v>
-      </c>
-      <c r="E64" t="s">
-        <v>43</v>
-      </c>
-      <c r="F64" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="B65" t="s">
-        <v>368</v>
-      </c>
-      <c r="C65" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" t="s">
-        <v>42</v>
-      </c>
-      <c r="E65" t="s">
-        <v>43</v>
-      </c>
-      <c r="F65" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" t="s">
-        <v>375</v>
-      </c>
-      <c r="C66" t="s">
-        <v>39</v>
-      </c>
-      <c r="D66" t="s">
-        <v>42</v>
-      </c>
-      <c r="E66" t="s">
-        <v>43</v>
-      </c>
-      <c r="F66" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="B67" t="s">
-        <v>379</v>
-      </c>
-      <c r="C67" t="s">
-        <v>40</v>
-      </c>
-      <c r="D67" t="s">
-        <v>42</v>
-      </c>
-      <c r="E67" t="s">
-        <v>43</v>
-      </c>
-      <c r="F67" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="B68" t="s">
-        <v>380</v>
-      </c>
-      <c r="C68" t="s">
-        <v>50</v>
-      </c>
-      <c r="D68" t="s">
-        <v>42</v>
-      </c>
-      <c r="E68" t="s">
-        <v>43</v>
-      </c>
-      <c r="F68" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="B69" t="s">
-        <v>382</v>
-      </c>
-      <c r="C69" t="s">
-        <v>37</v>
-      </c>
-      <c r="D69" t="s">
-        <v>54</v>
-      </c>
-      <c r="E69" t="s">
-        <v>43</v>
-      </c>
-      <c r="F69" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" t="s">
-        <v>384</v>
-      </c>
-      <c r="C70" t="s">
-        <v>37</v>
-      </c>
-      <c r="D70" t="s">
-        <v>54</v>
-      </c>
-      <c r="E70" t="s">
-        <v>43</v>
-      </c>
-      <c r="F70" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="71">
-      <c r="B71" t="s">
-        <v>398</v>
-      </c>
-      <c r="C71" t="s">
-        <v>325</v>
-      </c>
-      <c r="D71" t="s">
-        <v>54</v>
-      </c>
-      <c r="E71" t="s">
-        <v>43</v>
-      </c>
-      <c r="F71" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="B72" t="s">
-        <v>399</v>
-      </c>
-      <c r="C72" t="s">
-        <v>325</v>
-      </c>
-      <c r="D72" t="s">
-        <v>42</v>
-      </c>
-      <c r="E72" t="s">
-        <v>43</v>
-      </c>
-      <c r="F72" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="B73" t="s">
-        <v>400</v>
-      </c>
-      <c r="C73" t="s">
-        <v>325</v>
-      </c>
-      <c r="D73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E73" t="s">
-        <v>43</v>
-      </c>
-      <c r="F73" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="B74" t="s">
-        <v>401</v>
-      </c>
-      <c r="C74" t="s">
-        <v>325</v>
-      </c>
-      <c r="D74" t="s">
-        <v>42</v>
-      </c>
-      <c r="E74" t="s">
-        <v>43</v>
-      </c>
-      <c r="F74" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" t="s">
-        <v>402</v>
-      </c>
-      <c r="C75" t="s">
-        <v>325</v>
-      </c>
-      <c r="D75" t="s">
-        <v>54</v>
-      </c>
-      <c r="E75" t="s">
-        <v>43</v>
-      </c>
-      <c r="F75" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" t="s">
-        <v>403</v>
-      </c>
-      <c r="C76" t="s">
-        <v>325</v>
-      </c>
-      <c r="D76" t="s">
-        <v>42</v>
-      </c>
-      <c r="E76" t="s">
-        <v>43</v>
-      </c>
-      <c r="F76" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" t="s">
-        <v>404</v>
-      </c>
-      <c r="C77" t="s">
-        <v>325</v>
-      </c>
-      <c r="D77" t="s">
-        <v>54</v>
-      </c>
-      <c r="E77" t="s">
-        <v>43</v>
-      </c>
-      <c r="F77" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" t="s">
-        <v>405</v>
-      </c>
-      <c r="C78" t="s">
-        <v>325</v>
-      </c>
-      <c r="D78" t="s">
-        <v>42</v>
-      </c>
-      <c r="E78" t="s">
-        <v>43</v>
-      </c>
-      <c r="F78" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="B79" t="s">
-        <v>406</v>
-      </c>
-      <c r="C79" t="s">
-        <v>325</v>
-      </c>
-      <c r="D79" t="s">
-        <v>54</v>
-      </c>
-      <c r="E79" t="s">
-        <v>43</v>
-      </c>
-      <c r="F79" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="B80" t="s">
-        <v>407</v>
-      </c>
-      <c r="C80" t="s">
-        <v>325</v>
-      </c>
-      <c r="D80" t="s">
-        <v>42</v>
-      </c>
-      <c r="E80" t="s">
-        <v>43</v>
-      </c>
-      <c r="F80" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="B81" t="s">
-        <v>408</v>
-      </c>
-      <c r="C81" t="s">
-        <v>37</v>
-      </c>
-      <c r="D81" t="s">
-        <v>42</v>
-      </c>
-      <c r="E81" t="s">
-        <v>43</v>
-      </c>
-      <c r="F81" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="B82" t="s">
-        <v>409</v>
-      </c>
-      <c r="C82" t="s">
-        <v>40</v>
-      </c>
-      <c r="D82" t="s">
-        <v>42</v>
-      </c>
-      <c r="E82" t="s">
-        <v>43</v>
-      </c>
-      <c r="F82" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="B83" t="s">
-        <v>411</v>
-      </c>
-      <c r="C83" t="s">
-        <v>50</v>
-      </c>
-      <c r="D83" t="s">
-        <v>54</v>
-      </c>
-      <c r="E83" t="s">
-        <v>43</v>
-      </c>
-      <c r="F83" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="B84" t="s">
-        <v>413</v>
-      </c>
-      <c r="C84" t="s">
-        <v>40</v>
-      </c>
-      <c r="D84" t="s">
-        <v>42</v>
-      </c>
-      <c r="E84" t="s">
-        <v>43</v>
-      </c>
-      <c r="F84" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="B85" t="s">
-        <v>414</v>
-      </c>
-      <c r="C85" t="s">
-        <v>40</v>
-      </c>
-      <c r="D85" t="s">
-        <v>54</v>
-      </c>
-      <c r="E85" t="s">
-        <v>43</v>
-      </c>
-      <c r="F85" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="B86" t="s">
-        <v>416</v>
-      </c>
-      <c r="C86" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" t="s">
-        <v>54</v>
-      </c>
-      <c r="E86" t="s">
-        <v>43</v>
-      </c>
-      <c r="F86" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="B87" t="s">
-        <v>417</v>
-      </c>
-      <c r="C87" t="s">
-        <v>40</v>
-      </c>
-      <c r="D87" t="s">
-        <v>42</v>
-      </c>
-      <c r="E87" t="s">
-        <v>43</v>
-      </c>
-      <c r="F87" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="B88" t="s">
-        <v>418</v>
-      </c>
-      <c r="C88" t="s">
-        <v>40</v>
-      </c>
-      <c r="D88" t="s">
-        <v>54</v>
-      </c>
-      <c r="E88" t="s">
-        <v>43</v>
-      </c>
-      <c r="F88" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="B89" t="s">
-        <v>428</v>
-      </c>
-      <c r="C89" t="s">
-        <v>37</v>
-      </c>
-      <c r="D89" t="s">
-        <v>42</v>
-      </c>
-      <c r="E89" t="s">
-        <v>43</v>
-      </c>
-      <c r="F89" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="B90" t="s">
-        <v>429</v>
-      </c>
-      <c r="C90" t="s">
-        <v>40</v>
-      </c>
-      <c r="D90" t="s">
-        <v>42</v>
-      </c>
-      <c r="E90" t="s">
-        <v>43</v>
-      </c>
-      <c r="F90" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="B91" t="s">
-        <v>495</v>
-      </c>
-      <c r="C91" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" t="s">
-        <v>42</v>
-      </c>
-      <c r="E91" t="s">
-        <v>43</v>
-      </c>
-      <c r="F91" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="B92" t="s">
-        <v>496</v>
-      </c>
-      <c r="C92" t="s">
-        <v>50</v>
-      </c>
-      <c r="D92" t="s">
-        <v>42</v>
-      </c>
-      <c r="E92" t="s">
-        <v>43</v>
-      </c>
-      <c r="F92" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="B93" t="s">
-        <v>517</v>
-      </c>
-      <c r="C93" t="s">
-        <v>325</v>
-      </c>
-      <c r="D93" t="s">
-        <v>42</v>
-      </c>
-      <c r="E93" t="s">
-        <v>43</v>
-      </c>
-      <c r="F93" t="s">
-        <v>518</v>
-      </c>
-    </row>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
     <row r="94"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
modal resultados para envio
</commit_message>
<xml_diff>
--- a/SmartScale/assets/texts/texts.xlsx
+++ b/SmartScale/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111062" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119012" uniqueCount="684">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2355,6 +2355,108 @@
   </si>
   <si>
     <t xml:space="preserve">diferencia permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello my dudes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enviar Datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Enviar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos 
+Invalidos</t>
   </si>
 </sst>
 </file>
@@ -4083,75 +4185,75 @@
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>174</v>
+        <v>204</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>186</v>
+        <v>324</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>204</v>
+        <v>333</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -4163,15 +4265,15 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>162</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>205</v>
+        <v>335</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>325</v>
       </c>
       <c r="D14" t="s">
         <v>42</v>
@@ -4180,32 +4282,32 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>206</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
         <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>373</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
         <v>42</v>
@@ -4214,15 +4316,15 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>334</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C17" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
         <v>42</v>
@@ -4231,12 +4333,12 @@
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>94</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -4248,15 +4350,15 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>334</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
@@ -4265,32 +4367,32 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>340</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
@@ -4299,29 +4401,29 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>325</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>374</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="C23" t="s">
         <v>325</v>
@@ -4333,46 +4435,46 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>378</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="C24" t="s">
         <v>325</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>347</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="C25" t="s">
         <v>325</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>329</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C26" t="s">
         <v>325</v>
@@ -4389,7 +4491,7 @@
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C27" t="s">
         <v>325</v>
@@ -4406,58 +4508,58 @@
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C28" t="s">
         <v>325</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>360</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C29" t="s">
         <v>325</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E29" t="s">
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>94</v>
+        <v>360</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C30" t="s">
         <v>325</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="C31" t="s">
         <v>325</v>
@@ -4469,12 +4571,12 @@
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>360</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C32" t="s">
         <v>325</v>
@@ -4486,12 +4588,12 @@
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>360</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C33" t="s">
         <v>325</v>
@@ -4503,15 +4605,15 @@
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>326</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="C34" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -4520,15 +4622,15 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>326</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="C35" t="s">
-        <v>325</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
@@ -4537,15 +4639,15 @@
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="C36" t="s">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="D36" t="s">
         <v>42</v>
@@ -4554,15 +4656,15 @@
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
         <v>42</v>
@@ -4571,117 +4673,117 @@
         <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E38" t="s">
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>327</v>
+        <v>383</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E39" t="s">
         <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>369</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>380</v>
+        <v>596</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>381</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>382</v>
+        <v>597</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E41" t="s">
         <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>383</v>
+        <v>598</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>384</v>
+        <v>630</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E42" t="s">
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>126</v>
+        <v>631</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>596</v>
+        <v>632</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="D43" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E43" t="s">
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>185</v>
+        <v>633</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>597</v>
+        <v>634</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="D44" t="s">
         <v>42</v>
@@ -4690,49 +4792,49 @@
         <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>598</v>
+        <v>651</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>605</v>
+        <v>635</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>325</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E45" t="s">
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>606</v>
+        <v>652</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>607</v>
+        <v>637</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>325</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E46" t="s">
         <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>126</v>
+        <v>653</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
         <v>42</v>
@@ -4741,83 +4843,83 @@
         <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>631</v>
+        <v>646</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>325</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>642</v>
       </c>
       <c r="E48" t="s">
         <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>633</v>
+        <v>646</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="C49" t="s">
         <v>325</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>642</v>
       </c>
       <c r="E49" t="s">
         <v>43</v>
       </c>
       <c r="F49" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="C50" t="s">
         <v>325</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>642</v>
       </c>
       <c r="E50" t="s">
         <v>43</v>
       </c>
       <c r="F50" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="C51" t="s">
         <v>325</v>
       </c>
       <c r="D51" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E51" t="s">
         <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>653</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>639</v>
+        <v>647</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>325</v>
       </c>
       <c r="D52" t="s">
         <v>42</v>
@@ -4826,83 +4928,83 @@
         <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>646</v>
+        <v>369</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>641</v>
+        <v>648</v>
       </c>
       <c r="C53" t="s">
-        <v>325</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>642</v>
+        <v>42</v>
       </c>
       <c r="E53" t="s">
         <v>43</v>
       </c>
       <c r="F53" t="s">
-        <v>646</v>
+        <v>369</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="C54" t="s">
         <v>325</v>
       </c>
       <c r="D54" t="s">
-        <v>642</v>
+        <v>42</v>
       </c>
       <c r="E54" t="s">
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>646</v>
+        <v>369</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="C55" t="s">
         <v>325</v>
       </c>
       <c r="D55" t="s">
-        <v>642</v>
+        <v>42</v>
       </c>
       <c r="E55" t="s">
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>646</v>
+        <v>369</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="C56" t="s">
-        <v>325</v>
+        <v>167</v>
       </c>
       <c r="D56" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E56" t="s">
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>126</v>
+        <v>668</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>647</v>
+        <v>656</v>
       </c>
       <c r="C57" t="s">
-        <v>325</v>
+        <v>37</v>
       </c>
       <c r="D57" t="s">
         <v>42</v>
@@ -4911,15 +5013,15 @@
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>369</v>
+        <v>633</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>648</v>
+        <v>657</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>325</v>
       </c>
       <c r="D58" t="s">
         <v>42</v>
@@ -4928,12 +5030,12 @@
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>369</v>
+        <v>651</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
       <c r="C59" t="s">
         <v>325</v>
@@ -4945,12 +5047,12 @@
         <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>369</v>
+        <v>652</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>650</v>
+        <v>659</v>
       </c>
       <c r="C60" t="s">
         <v>325</v>
@@ -4962,19 +5064,179 @@
         <v>43</v>
       </c>
       <c r="F60" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>660</v>
+      </c>
+      <c r="C61" t="s">
+        <v>37</v>
+      </c>
+      <c r="D61" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" t="s">
+        <v>43</v>
+      </c>
+      <c r="F61" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>661</v>
+      </c>
+      <c r="C62" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62" t="s">
+        <v>43</v>
+      </c>
+      <c r="F62" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>662</v>
+      </c>
+      <c r="C63" t="s">
+        <v>325</v>
+      </c>
+      <c r="D63" t="s">
+        <v>642</v>
+      </c>
+      <c r="E63" t="s">
+        <v>43</v>
+      </c>
+      <c r="F63" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>663</v>
+      </c>
+      <c r="C64" t="s">
+        <v>325</v>
+      </c>
+      <c r="D64" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" t="s">
+        <v>43</v>
+      </c>
+      <c r="F64" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>664</v>
+      </c>
+      <c r="C65" t="s">
+        <v>325</v>
+      </c>
+      <c r="D65" t="s">
+        <v>642</v>
+      </c>
+      <c r="E65" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>665</v>
+      </c>
+      <c r="C66" t="s">
+        <v>325</v>
+      </c>
+      <c r="D66" t="s">
+        <v>42</v>
+      </c>
+      <c r="E66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>666</v>
+      </c>
+      <c r="C67" t="s">
+        <v>325</v>
+      </c>
+      <c r="D67" t="s">
+        <v>642</v>
+      </c>
+      <c r="E67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>667</v>
+      </c>
+      <c r="C68" t="s">
+        <v>325</v>
+      </c>
+      <c r="D68" t="s">
+        <v>42</v>
+      </c>
+      <c r="E68" t="s">
+        <v>43</v>
+      </c>
+      <c r="F68" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>669</v>
+      </c>
+      <c r="C69" t="s">
+        <v>325</v>
+      </c>
+      <c r="D69" t="s">
+        <v>54</v>
+      </c>
+      <c r="E69" t="s">
+        <v>43</v>
+      </c>
+      <c r="F69" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>671</v>
+      </c>
+      <c r="C70" t="s">
+        <v>325</v>
+      </c>
+      <c r="D70" t="s">
+        <v>42</v>
+      </c>
+      <c r="E70" t="s">
+        <v>43</v>
+      </c>
+      <c r="F70" t="s">
+        <v>683</v>
+      </c>
+    </row>
     <row r="71"/>
     <row r="72"/>
     <row r="73"/>

</xml_diff>